<commit_message>
modifications des heures de nos taches
</commit_message>
<xml_diff>
--- a/taches.xlsx
+++ b/taches.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="600" windowWidth="17256" windowHeight="5772"/>
+    <workbookView xWindow="0" yWindow="1200" windowWidth="17256" windowHeight="5772"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -466,7 +466,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D11" sqref="D11"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -506,14 +508,14 @@
         <v>44656</v>
       </c>
       <c r="D2" s="4">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="E2" s="4" t="s">
         <v>26</v>
       </c>
       <c r="F2" s="5">
         <f>SUM(C2:D2)</f>
-        <v>44660</v>
+        <v>44662</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -525,7 +527,7 @@
       </c>
       <c r="C3" s="5">
         <f>SUM(C2,D2)</f>
-        <v>44660</v>
+        <v>44662</v>
       </c>
       <c r="D3" s="4">
         <v>3</v>
@@ -535,7 +537,7 @@
       </c>
       <c r="F3" s="5">
         <f t="shared" ref="F3:F11" si="0">SUM(C3:D3)</f>
-        <v>44663</v>
+        <v>44665</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -547,7 +549,7 @@
       </c>
       <c r="C4" s="5">
         <f t="shared" ref="C4:C11" si="1">SUM(C3,D3)</f>
-        <v>44663</v>
+        <v>44665</v>
       </c>
       <c r="D4" s="4">
         <v>2</v>
@@ -557,7 +559,7 @@
       </c>
       <c r="F4" s="5">
         <f t="shared" si="0"/>
-        <v>44665</v>
+        <v>44667</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -569,7 +571,7 @@
       </c>
       <c r="C5" s="5">
         <f t="shared" si="1"/>
-        <v>44665</v>
+        <v>44667</v>
       </c>
       <c r="D5" s="4">
         <v>2</v>
@@ -579,7 +581,7 @@
       </c>
       <c r="F5" s="5">
         <f t="shared" si="0"/>
-        <v>44667</v>
+        <v>44669</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -591,7 +593,7 @@
       </c>
       <c r="C6" s="5">
         <f t="shared" si="1"/>
-        <v>44667</v>
+        <v>44669</v>
       </c>
       <c r="D6" s="4">
         <v>2</v>
@@ -601,7 +603,7 @@
       </c>
       <c r="F6" s="5">
         <f t="shared" si="0"/>
-        <v>44669</v>
+        <v>44671</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -613,17 +615,17 @@
       </c>
       <c r="C7" s="5">
         <f t="shared" si="1"/>
-        <v>44669</v>
+        <v>44671</v>
       </c>
       <c r="D7" s="4">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E7" s="4" t="s">
         <v>17</v>
       </c>
       <c r="F7" s="5">
         <f t="shared" si="0"/>
-        <v>44671</v>
+        <v>44674</v>
       </c>
     </row>
     <row r="8" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -635,17 +637,17 @@
       </c>
       <c r="C8" s="5">
         <f t="shared" si="1"/>
-        <v>44671</v>
+        <v>44674</v>
       </c>
       <c r="D8" s="4">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E8" s="4" t="s">
         <v>22</v>
       </c>
       <c r="F8" s="5">
         <f t="shared" si="0"/>
-        <v>44673</v>
+        <v>44677</v>
       </c>
     </row>
     <row r="9" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -657,7 +659,7 @@
       </c>
       <c r="C9" s="5">
         <f t="shared" si="1"/>
-        <v>44673</v>
+        <v>44677</v>
       </c>
       <c r="D9" s="4">
         <v>2</v>
@@ -667,7 +669,7 @@
       </c>
       <c r="F9" s="5">
         <f t="shared" si="0"/>
-        <v>44675</v>
+        <v>44679</v>
       </c>
     </row>
     <row r="10" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -679,7 +681,7 @@
       </c>
       <c r="C10" s="5">
         <f t="shared" si="1"/>
-        <v>44675</v>
+        <v>44679</v>
       </c>
       <c r="D10" s="4">
         <v>9</v>
@@ -689,7 +691,7 @@
       </c>
       <c r="F10" s="5">
         <f t="shared" si="0"/>
-        <v>44684</v>
+        <v>44688</v>
       </c>
     </row>
     <row r="11" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -701,17 +703,17 @@
       </c>
       <c r="C11" s="5">
         <f t="shared" si="1"/>
-        <v>44684</v>
+        <v>44688</v>
       </c>
       <c r="D11" s="4">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="E11" s="4" t="s">
         <v>24</v>
       </c>
       <c r="F11" s="5">
         <f t="shared" si="0"/>
-        <v>44686</v>
+        <v>44692</v>
       </c>
     </row>
   </sheetData>

</xml_diff>